<commit_message>
Comparing human data with HDC and McRae..
</commit_message>
<xml_diff>
--- a/CompareHumanData/ExperimentalResults.xlsx
+++ b/CompareHumanData/ExperimentalResults.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jobqu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\CompareHumanData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E5C03A10-1B9A-4455-A2D9-29A3F9847B16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB737827-DF03-4310-B144-2990FB7EEA44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="9583" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,15 +18,15 @@
     <sheet name="Results" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparison!$A$1:$D$69</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparison!$A$1:$D$66</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Summary!$A$1:$C$69</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="236">
   <si>
     <t>Timestamp</t>
   </si>
@@ -565,205 +565,175 @@
     <t>concept 2</t>
   </si>
   <si>
-    <t xml:space="preserve">spoon </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> barrel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shoes </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bike</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> truck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chair </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pen</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> envelope</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> whip</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> box</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> shield</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> book</t>
-  </si>
-  <si>
-    <t xml:space="preserve">table </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> brush</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> basket</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> curtains</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ashtray</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> car</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> lamp</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carpet </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> scarf</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> carpet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bed </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> knife</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> closet</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> earmuffs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> wardrobe</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> dresser</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> spoon</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> skirt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bookcase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bowl </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bathtub</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> chair</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> colander</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> belt</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sofa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boots </t>
-  </si>
-  <si>
-    <t xml:space="preserve">pen </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pijama</t>
-  </si>
-  <si>
-    <t xml:space="preserve">stove </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pot</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bench</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cushion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shovel </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> machete</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> tongs</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> spatula</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> plate</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> pillow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">knife </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> scissors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dresser </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> socks</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> desk</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cup </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bottle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">skirt </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> trousers</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sandal</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fork</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> slipper</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> rocker</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ladle</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> boots</t>
-  </si>
-  <si>
     <t>mink_(coat)</t>
+  </si>
+  <si>
+    <t>spoon</t>
+  </si>
+  <si>
+    <t>shoes</t>
+  </si>
+  <si>
+    <t>chair</t>
+  </si>
+  <si>
+    <t>table</t>
+  </si>
+  <si>
+    <t>carpet</t>
+  </si>
+  <si>
+    <t>bed</t>
+  </si>
+  <si>
+    <t>bowl</t>
+  </si>
+  <si>
+    <t>boots</t>
+  </si>
+  <si>
+    <t>pen</t>
+  </si>
+  <si>
+    <t>stove</t>
+  </si>
+  <si>
+    <t>shovel</t>
+  </si>
+  <si>
+    <t>knife</t>
+  </si>
+  <si>
+    <t>dresser</t>
+  </si>
+  <si>
+    <t>cup</t>
+  </si>
+  <si>
+    <t>skirt</t>
+  </si>
+  <si>
+    <t>barrel</t>
+  </si>
+  <si>
+    <t>bike</t>
+  </si>
+  <si>
+    <t>truck</t>
+  </si>
+  <si>
+    <t>envelope</t>
+  </si>
+  <si>
+    <t>whip</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>shield</t>
+  </si>
+  <si>
+    <t>book</t>
+  </si>
+  <si>
+    <t>brush</t>
+  </si>
+  <si>
+    <t>basket</t>
+  </si>
+  <si>
+    <t>curtains</t>
+  </si>
+  <si>
+    <t>ashtray</t>
+  </si>
+  <si>
+    <t>car</t>
+  </si>
+  <si>
+    <t>lamp</t>
+  </si>
+  <si>
+    <t>scarf</t>
+  </si>
+  <si>
+    <t>closet</t>
+  </si>
+  <si>
+    <t>earmuffs</t>
+  </si>
+  <si>
+    <t>bookcase</t>
+  </si>
+  <si>
+    <t>bathtub</t>
+  </si>
+  <si>
+    <t>colander</t>
+  </si>
+  <si>
+    <t>belt</t>
+  </si>
+  <si>
+    <t>sofa</t>
+  </si>
+  <si>
+    <t>pot</t>
+  </si>
+  <si>
+    <t>bench</t>
+  </si>
+  <si>
+    <t>cushion</t>
+  </si>
+  <si>
+    <t>machete</t>
+  </si>
+  <si>
+    <t>tongs</t>
+  </si>
+  <si>
+    <t>spatula</t>
+  </si>
+  <si>
+    <t>plate</t>
+  </si>
+  <si>
+    <t>pillow</t>
+  </si>
+  <si>
+    <t>scissors</t>
+  </si>
+  <si>
+    <t>socks</t>
+  </si>
+  <si>
+    <t>desk</t>
+  </si>
+  <si>
+    <t>bottle</t>
+  </si>
+  <si>
+    <t>trousers</t>
+  </si>
+  <si>
+    <t>fork</t>
+  </si>
+  <si>
+    <t>rocker</t>
+  </si>
+  <si>
+    <t>ladle</t>
+  </si>
+  <si>
+    <t>pajamas</t>
+  </si>
+  <si>
+    <t>sandals</t>
+  </si>
+  <si>
+    <t>slippers</t>
   </si>
 </sst>
 </file>
@@ -1247,7 +1217,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1257,9 +1227,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1617,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEE3531-55C1-47A9-B36A-220313F45DAE}">
-  <dimension ref="A1:D69"/>
+  <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -1647,10 +1614,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="C2" s="4">
         <v>1</v>
@@ -1664,7 +1631,7 @@
         <v>181</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
       <c r="C3" s="4">
         <v>1.0666666666666667</v>
@@ -1675,10 +1642,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>183</v>
+        <v>197</v>
       </c>
       <c r="C4" s="4">
         <v>1.0666666666666667</v>
@@ -1689,10 +1656,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C5" s="4">
         <v>1.1000000000000001</v>
@@ -1703,10 +1670,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>186</v>
+        <v>198</v>
       </c>
       <c r="C6" s="4">
         <v>1.1000000000000001</v>
@@ -1720,7 +1687,7 @@
         <v>181</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="C7" s="4">
         <v>1.1666666666666667</v>
@@ -1731,10 +1698,10 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="C8" s="4">
         <v>1.2</v>
@@ -1748,7 +1715,7 @@
         <v>181</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>189</v>
+        <v>201</v>
       </c>
       <c r="C9" s="4">
         <v>1.2333333333333334</v>
@@ -1759,10 +1726,10 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>190</v>
+        <v>202</v>
       </c>
       <c r="C10" s="4">
         <v>1.2666666666666666</v>
@@ -1773,10 +1740,10 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>192</v>
+        <v>203</v>
       </c>
       <c r="C11" s="4">
         <v>1.3</v>
@@ -1787,10 +1754,10 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>193</v>
+        <v>204</v>
       </c>
       <c r="C12" s="4">
         <v>1.3333333333333333</v>
@@ -1801,10 +1768,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>194</v>
+        <v>205</v>
       </c>
       <c r="C13" s="4">
         <v>1.6333333333333333</v>
@@ -1815,10 +1782,10 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>195</v>
+        <v>206</v>
       </c>
       <c r="C14" s="4">
         <v>1.6333333333333333</v>
@@ -1829,10 +1796,10 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>180</v>
+        <v>195</v>
       </c>
       <c r="C15" s="4">
         <v>1.7333333333333334</v>
@@ -1843,10 +1810,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C16" s="4">
         <v>1.8333333333333333</v>
@@ -1857,10 +1824,10 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C17" s="4">
         <v>1.9333333333333333</v>
@@ -1871,10 +1838,10 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>199</v>
+        <v>209</v>
       </c>
       <c r="C18" s="4">
         <v>1.9666666666666666</v>
@@ -1888,7 +1855,7 @@
         <v>181</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="C19" s="4">
         <v>2</v>
@@ -1899,10 +1866,10 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>197</v>
+        <v>208</v>
       </c>
       <c r="C20" s="4">
         <v>2.0666666666666669</v>
@@ -1913,10 +1880,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>245</v>
+        <v>179</v>
       </c>
       <c r="C21" s="4">
         <v>2.1</v>
@@ -1927,10 +1894,10 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="C22" s="4">
         <v>2.1</v>
@@ -1941,10 +1908,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C23" s="4">
         <v>2.2333333333333334</v>
@@ -1958,7 +1925,7 @@
         <v>181</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="C24" s="4">
         <v>2.2666666666666666</v>
@@ -1968,535 +1935,535 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C25" s="5">
+      <c r="A25" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C25" s="4">
         <v>2.2999999999999998</v>
       </c>
-      <c r="D25" s="5">
-        <v>1.6563010998406458</v>
+      <c r="D25" s="4">
+        <v>1.6763054614240209</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="C26" s="4">
-        <v>2.2999999999999998</v>
+        <v>2.3333333333333335</v>
       </c>
       <c r="D26" s="4">
-        <v>1.6763054614240209</v>
+        <v>2.3428377854407438</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C27" s="4">
-        <v>2.3333333333333335</v>
+        <v>2.4</v>
       </c>
       <c r="D27" s="4">
-        <v>2.3428377854407438</v>
+        <v>1.5832456116050557</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C28" s="4">
-        <v>2.4</v>
+        <v>2.4333333333333331</v>
       </c>
       <c r="D28" s="4">
-        <v>1.5832456116050557</v>
+        <v>1.8917951498216947</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C29" s="4">
-        <v>2.4333333333333331</v>
+        <v>2.4666666666666668</v>
       </c>
       <c r="D29" s="4">
-        <v>1.8917951498216947</v>
+        <v>1.6275407487644937</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>209</v>
+        <v>179</v>
       </c>
       <c r="C30" s="4">
         <v>2.4666666666666668</v>
       </c>
       <c r="D30" s="4">
-        <v>1.6275407487644937</v>
+        <v>1.7461067804945061</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
       <c r="C31" s="4">
-        <v>2.4666666666666668</v>
+        <v>2.5333333333333332</v>
       </c>
       <c r="D31" s="4">
-        <v>1.7461067804945061</v>
+        <v>1.564892612574067</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="C32" s="4">
-        <v>2.5333333333333332</v>
+        <v>2.6333333333333333</v>
       </c>
       <c r="D32" s="4">
-        <v>1.564892612574067</v>
+        <v>1.8162843634433703</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C33" s="4">
+        <v>2.7333333333333334</v>
+      </c>
+      <c r="D33" s="4">
+        <v>1.9988885800753267</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C33" s="4">
-        <v>2.6333333333333333</v>
-      </c>
-      <c r="D33" s="4">
-        <v>1.8162843634433703</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C34" s="5">
-        <v>2.7</v>
-      </c>
-      <c r="D34" s="5">
-        <v>1.5088627063675035</v>
+      <c r="C34" s="4">
+        <v>2.9333333333333331</v>
+      </c>
+      <c r="D34" s="4">
+        <v>1.6918103387266026</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C35" s="4">
-        <v>2.7333333333333334</v>
+        <v>2.9333333333333331</v>
       </c>
       <c r="D35" s="4">
-        <v>1.9988885800753267</v>
+        <v>1.8061622912192088</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="C36" s="4">
-        <v>2.9333333333333331</v>
+        <v>3.0333333333333332</v>
       </c>
       <c r="D36" s="4">
-        <v>1.6918103387266026</v>
+        <v>2.1052843566184172</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>213</v>
+        <v>192</v>
       </c>
       <c r="C37" s="4">
-        <v>2.9333333333333331</v>
+        <v>3.0666666666666669</v>
       </c>
       <c r="D37" s="4">
-        <v>1.8061622912192088</v>
+        <v>1.8607047649270483</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C38" s="4">
-        <v>3.0333333333333332</v>
+        <v>3.0666666666666669</v>
       </c>
       <c r="D38" s="4">
-        <v>2.1052843566184172</v>
+        <v>2.1746008573733455</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>206</v>
+        <v>183</v>
       </c>
       <c r="C39" s="4">
-        <v>3.0666666666666669</v>
+        <v>3.1333333333333333</v>
       </c>
       <c r="D39" s="4">
-        <v>1.8607047649270483</v>
+        <v>1.7650936393164969</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>215</v>
       </c>
       <c r="C40" s="4">
-        <v>3.0666666666666669</v>
+        <v>3.1333333333333333</v>
       </c>
       <c r="D40" s="4">
-        <v>2.1746008573733455</v>
+        <v>1.8749814813900312</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>201</v>
+        <v>188</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>216</v>
+        <v>198</v>
       </c>
       <c r="C41" s="4">
-        <v>3.1333333333333333</v>
+        <v>3.4</v>
       </c>
       <c r="D41" s="4">
-        <v>1.7650936393164969</v>
+        <v>2.5638512697372549</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>214</v>
+        <v>233</v>
       </c>
       <c r="C42" s="4">
-        <v>3.1333333333333333</v>
+        <v>3.8666666666666667</v>
       </c>
       <c r="D42" s="4">
-        <v>1.8749814813900312</v>
+        <v>2.3907228102721478</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
-        <v>218</v>
+        <v>189</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>186</v>
+        <v>217</v>
       </c>
       <c r="C43" s="4">
-        <v>3.4</v>
+        <v>3.9</v>
       </c>
       <c r="D43" s="4">
-        <v>2.5638512697372549</v>
+        <v>2.2412793965352318</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
-        <v>201</v>
+        <v>183</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C44" s="4">
-        <v>3.8666666666666667</v>
+        <v>4</v>
       </c>
       <c r="D44" s="4">
-        <v>2.3907228102721478</v>
+        <v>2.5690465157330258</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
-        <v>220</v>
+        <v>185</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C45" s="4">
-        <v>3.9</v>
+        <v>4.0999999999999996</v>
       </c>
       <c r="D45" s="4">
-        <v>2.2412793965352318</v>
+        <v>2.3144473782453265</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C46" s="4">
-        <v>4</v>
+        <v>4.1333333333333337</v>
       </c>
       <c r="D46" s="4">
-        <v>2.5690465157330258</v>
+        <v>2.3342855200015462</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
-        <v>201</v>
+        <v>182</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>223</v>
+        <v>183</v>
       </c>
       <c r="C47" s="4">
-        <v>4.0999999999999996</v>
+        <v>4.3666666666666663</v>
       </c>
       <c r="D47" s="4">
-        <v>2.3144473782453265</v>
+        <v>2.4695928589321943</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>224</v>
+        <v>183</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="C48" s="4">
-        <v>4.1333333333333337</v>
+        <v>4.4333333333333336</v>
       </c>
       <c r="D48" s="4">
-        <v>2.3342855200015462</v>
+        <v>2.2313423961572747</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>216</v>
+        <v>221</v>
       </c>
       <c r="C49" s="4">
-        <v>4.3666666666666663</v>
+        <v>4.4333333333333336</v>
       </c>
       <c r="D49" s="4">
-        <v>2.4695928589321943</v>
+        <v>2.5907956735764057</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="C50" s="4">
-        <v>4.4333333333333336</v>
+        <v>4.5333333333333332</v>
       </c>
       <c r="D50" s="4">
-        <v>2.2313423961572747</v>
+        <v>2.777688887466621</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C51" s="4">
-        <v>4.4333333333333336</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="D51" s="4">
-        <v>2.5907956735764057</v>
+        <v>2.6718699236468995</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>215</v>
+        <v>223</v>
       </c>
       <c r="C52" s="4">
-        <v>4.5333333333333332</v>
+        <v>5</v>
       </c>
       <c r="D52" s="4">
-        <v>2.777688887466621</v>
+        <v>2.6708300832013507</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C53" s="4">
-        <v>4.833333333333333</v>
+        <v>5.1333333333333337</v>
       </c>
       <c r="D53" s="4">
-        <v>2.6718699236468995</v>
+        <v>2.6674998698323411</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>179</v>
+        <v>191</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C54" s="4">
-        <v>5</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="D54" s="4">
-        <v>2.6708300832013507</v>
+        <v>2.3392781412697001</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>201</v>
+        <v>181</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="C55" s="4">
-        <v>5.1333333333333337</v>
+        <v>5.3666666666666663</v>
       </c>
       <c r="D55" s="4">
-        <v>2.6674998698323411</v>
+        <v>2.5492918406665193</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>230</v>
+        <v>183</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C56" s="4">
-        <v>5.166666666666667</v>
+        <v>5.3666666666666663</v>
       </c>
       <c r="D56" s="4">
-        <v>2.3392781412697001</v>
+        <v>2.8807792155749961</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="B57" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="C57" s="5">
-        <v>5.3</v>
-      </c>
-      <c r="D57" s="5">
-        <v>2.6602004936971699</v>
+      <c r="A57" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C57" s="4">
+        <v>5.4333333333333336</v>
+      </c>
+      <c r="D57" s="4">
+        <v>2.848196310337864</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C58" s="4">
-        <v>5.3666666666666663</v>
+        <v>5.5333333333333332</v>
       </c>
       <c r="D58" s="4">
-        <v>2.5492918406665193</v>
+        <v>2.5914388967435746</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>234</v>
+        <v>216</v>
       </c>
       <c r="C59" s="4">
-        <v>5.3666666666666663</v>
+        <v>5.5333333333333332</v>
       </c>
       <c r="D59" s="4">
-        <v>2.8807792155749961</v>
+        <v>3.0630413353760377</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>235</v>
+        <v>181</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="C60" s="4">
-        <v>5.4333333333333336</v>
+        <v>5.7</v>
       </c>
       <c r="D60" s="4">
-        <v>2.848196310337864</v>
+        <v>3.2057240471797734</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>237</v>
+        <v>182</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>238</v>
+        <v>218</v>
       </c>
       <c r="C61" s="4">
-        <v>5.5333333333333332</v>
+        <v>5.9333333333333336</v>
       </c>
       <c r="D61" s="4">
-        <v>2.5914388967435746</v>
+        <v>2.8744081516413464</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="C62" s="4">
-        <v>5.5333333333333332</v>
+        <v>6.1333333333333337</v>
       </c>
       <c r="D62" s="4">
-        <v>3.0630413353760377</v>
+        <v>2.765662468358872</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2504,41 +2471,41 @@
         <v>181</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C63" s="4">
-        <v>5.7</v>
+        <v>6.1333333333333337</v>
       </c>
       <c r="D63" s="4">
-        <v>3.2057240471797734</v>
+        <v>3.2117838587855747</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="C64" s="4">
-        <v>5.9333333333333336</v>
+        <v>6.4</v>
       </c>
       <c r="D64" s="4">
-        <v>2.8744081516413464</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="C65" s="4">
-        <v>6.1333333333333337</v>
+        <v>6.5</v>
       </c>
       <c r="D65" s="4">
-        <v>2.765662468358872</v>
+        <v>3.0849095070466275</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2546,54 +2513,12 @@
         <v>181</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>241</v>
+        <v>187</v>
       </c>
       <c r="C66" s="4">
-        <v>6.1333333333333337</v>
+        <v>6.7</v>
       </c>
       <c r="D66" s="4">
-        <v>3.2117838587855747</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="B67" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="C67" s="4">
-        <v>6.4</v>
-      </c>
-      <c r="D67" s="4">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="B68" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="C68" s="4">
-        <v>6.5</v>
-      </c>
-      <c r="D68" s="4">
-        <v>3.0849095070466275</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B69" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="C69" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="D69" s="4">
         <v>2.9569128044860125</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Finish correlation between metrics
</commit_message>
<xml_diff>
--- a/CompareHumanData/ExperimentalResults.xlsx
+++ b/CompareHumanData/ExperimentalResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\CompareHumanData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB737827-DF03-4310-B144-2990FB7EEA44}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3943666-7A14-4DA3-BC82-28A80B138687}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="9583" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1586,8 +1586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEE3531-55C1-47A9-B36A-220313F45DAE}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B64" sqref="B64"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -2531,8 +2531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C69"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection sqref="A1:C56"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
small changes to excel reading function..
</commit_message>
<xml_diff>
--- a/CompareHumanData/ExperimentalResults.xlsx
+++ b/CompareHumanData/ExperimentalResults.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\JupyterN\VectorSymbolicArchitectures\CompareHumanData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3943666-7A14-4DA3-BC82-28A80B138687}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F64A576E-1A37-4095-A8C9-7301841BF0D3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25135" windowHeight="9583" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
     <sheet name="Results" sheetId="1" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparison!$A$1:$D$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Comparison!$A$1:$D$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Summary!$A$1:$C$69</definedName>
   </definedNames>
   <calcPr calcId="162913" concurrentCalc="0"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="236">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1584,10 +1584,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AEE3531-55C1-47A9-B36A-220313F45DAE}">
-  <dimension ref="A1:D66"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:XFD47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -2244,58 +2244,58 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="B47" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="B47" s="2" t="s">
-        <v>183</v>
-      </c>
       <c r="C47" s="4">
-        <v>4.3666666666666663</v>
+        <v>4.4333333333333336</v>
       </c>
       <c r="D47" s="4">
-        <v>2.4695928589321943</v>
+        <v>2.2313423961572747</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>182</v>
+        <v>221</v>
       </c>
       <c r="C48" s="4">
         <v>4.4333333333333336</v>
       </c>
       <c r="D48" s="4">
-        <v>2.2313423961572747</v>
+        <v>2.5907956735764057</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C49" s="4">
-        <v>4.4333333333333336</v>
+        <v>4.5333333333333332</v>
       </c>
       <c r="D49" s="4">
-        <v>2.5907956735764057</v>
+        <v>2.777688887466621</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="C50" s="4">
-        <v>4.5333333333333332</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="D50" s="4">
-        <v>2.777688887466621</v>
+        <v>2.6718699236468995</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -2303,222 +2303,208 @@
         <v>180</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="C51" s="4">
-        <v>4.833333333333333</v>
+        <v>5</v>
       </c>
       <c r="D51" s="4">
-        <v>2.6718699236468995</v>
+        <v>2.6708300832013507</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52" s="2" t="s">
-        <v>180</v>
+        <v>185</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C52" s="4">
-        <v>5</v>
+        <v>5.1333333333333337</v>
       </c>
       <c r="D52" s="4">
-        <v>2.6708300832013507</v>
+        <v>2.6674998698323411</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A53" s="2" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C53" s="4">
-        <v>5.1333333333333337</v>
+        <v>5.166666666666667</v>
       </c>
       <c r="D53" s="4">
-        <v>2.6674998698323411</v>
+        <v>2.3392781412697001</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54" s="2" t="s">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C54" s="4">
-        <v>5.166666666666667</v>
+        <v>5.3666666666666663</v>
       </c>
       <c r="D54" s="4">
-        <v>2.3392781412697001</v>
+        <v>2.5492918406665193</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C55" s="4">
         <v>5.3666666666666663</v>
       </c>
       <c r="D55" s="4">
-        <v>2.5492918406665193</v>
+        <v>2.8807792155749961</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A56" s="2" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C56" s="4">
-        <v>5.3666666666666663</v>
+        <v>5.4333333333333336</v>
       </c>
       <c r="D56" s="4">
-        <v>2.8807792155749961</v>
+        <v>2.848196310337864</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A57" s="2" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C57" s="4">
-        <v>5.4333333333333336</v>
+        <v>5.5333333333333332</v>
       </c>
       <c r="D57" s="4">
-        <v>2.848196310337864</v>
+        <v>2.5914388967435746</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A58" s="2" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>229</v>
+        <v>216</v>
       </c>
       <c r="C58" s="4">
         <v>5.5333333333333332</v>
       </c>
       <c r="D58" s="4">
-        <v>2.5914388967435746</v>
+        <v>3.0630413353760377</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A59" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>216</v>
+        <v>234</v>
       </c>
       <c r="C59" s="4">
-        <v>5.5333333333333332</v>
+        <v>5.7</v>
       </c>
       <c r="D59" s="4">
-        <v>3.0630413353760377</v>
+        <v>3.2057240471797734</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A60" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>234</v>
+        <v>218</v>
       </c>
       <c r="C60" s="4">
-        <v>5.7</v>
+        <v>5.9333333333333336</v>
       </c>
       <c r="D60" s="4">
-        <v>3.2057240471797734</v>
+        <v>2.8744081516413464</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="C61" s="4">
-        <v>5.9333333333333336</v>
+        <v>6.1333333333333337</v>
       </c>
       <c r="D61" s="4">
-        <v>2.8744081516413464</v>
+        <v>2.765662468358872</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A62" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>230</v>
+        <v>235</v>
       </c>
       <c r="C62" s="4">
         <v>6.1333333333333337</v>
       </c>
       <c r="D62" s="4">
-        <v>2.765662468358872</v>
+        <v>3.2117838587855747</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A63" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C63" s="4">
-        <v>6.1333333333333337</v>
+        <v>6.4</v>
       </c>
       <c r="D63" s="4">
-        <v>3.2117838587855747</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A64" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="C64" s="4">
-        <v>6.4</v>
+        <v>6.5</v>
       </c>
       <c r="D64" s="4">
-        <v>2.8</v>
+        <v>3.0849095070466275</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A65" s="2" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>232</v>
+        <v>187</v>
       </c>
       <c r="C65" s="4">
-        <v>6.5</v>
+        <v>6.7</v>
       </c>
       <c r="D65" s="4">
-        <v>3.0849095070466275</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>181</v>
-      </c>
-      <c r="B66" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="C66" s="4">
-        <v>6.7</v>
-      </c>
-      <c r="D66" s="4">
         <v>2.9569128044860125</v>
       </c>
     </row>

</xml_diff>